<commit_message>
Added Pre-Covid attendance and tidy up
</commit_message>
<xml_diff>
--- a/data/MyData.xlsx
+++ b/data/MyData.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://studentlit-my.sharepoint.com/personal/elaine_tynan_lit_ie/Documents/HDip/Semester2/ProgDataAnlys/repos/PfDA_Assignment/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://studentlit-my.sharepoint.com/personal/elaine_tynan_lit_ie/Documents/HDip/Semester2/ProgDataAnlys/repos/PfDA_Assignment/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="15" documentId="13_ncr:1_{23D08EC2-E12C-48CE-B319-7B75B59D63AF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{178D4A8D-28CD-41EF-B8F8-F006D1EED424}"/>
+  <xr:revisionPtr revIDLastSave="34" documentId="13_ncr:1_{23D08EC2-E12C-48CE-B319-7B75B59D63AF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F5C12870-61C4-4647-AAA1-75C426052053}"/>
   <bookViews>
-    <workbookView xWindow="1950" yWindow="1950" windowWidth="21600" windowHeight="11385" xr2:uid="{4E9EE3A0-650C-4A55-AEF7-713742751E40}"/>
+    <workbookView xWindow="780" yWindow="780" windowWidth="17070" windowHeight="11385" xr2:uid="{4E9EE3A0-650C-4A55-AEF7-713742751E40}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -918,7 +918,7 @@
   <dimension ref="A1:J189"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H110" sqref="H110"/>
+      <selection activeCell="L1" sqref="L1:O13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>